<commit_message>
refactor wifi and eeprom
</commit_message>
<xml_diff>
--- a/layout/layout.xlsx
+++ b/layout/layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roland\CloudStation\projects\arduino\co2_wifi\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09585D1-018C-49DA-A9B3-EABB2A6D4AB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF3AE62-5106-48A4-A749-89F78C0A718B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{3AD7B8E2-3131-40F9-960B-9A336FFF910D}"/>
+    <workbookView xWindow="34425" yWindow="510" windowWidth="17025" windowHeight="21000" xr2:uid="{3AD7B8E2-3131-40F9-960B-9A336FFF910D}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1656,7 +1656,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="27" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="26" width="3" style="1" customWidth="1"/>
     <col min="27" max="27" width="3.42578125" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
I2C screen and influx / grafana database
</commit_message>
<xml_diff>
--- a/layout/layout.xlsx
+++ b/layout/layout.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roland\CloudStation\projects\arduino\co2_wifi\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF3AE62-5106-48A4-A749-89F78C0A718B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F83F1BB-BE3B-4A34-A263-148329FAEF24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34425" yWindow="510" windowWidth="17025" windowHeight="21000" xr2:uid="{3AD7B8E2-3131-40F9-960B-9A336FFF910D}"/>
+    <workbookView xWindow="18270" yWindow="0" windowWidth="28320" windowHeight="20685" activeTab="1" xr2:uid="{3AD7B8E2-3131-40F9-960B-9A336FFF910D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="V1 SPI" sheetId="1" r:id="rId1"/>
+    <sheet name="V2 I2C" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="36">
   <si>
     <t>A</t>
   </si>
@@ -1351,6 +1352,882 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>124562</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>124558</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>32813</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>175850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Afbeelding 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ACD36D5-1C4C-4CB9-80E6-0BAC4020D11F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:alphaModFix amt="58000"/>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="214966" y="6053954"/>
+          <a:ext cx="2537317" cy="1537026"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>21984</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>14653</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>62120</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Afbeelding 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EA613F8-56D9-4013-9C58-7F9FCFDB52AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:alphaModFix amt="58000"/>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3241719" y="604918"/>
+          <a:ext cx="1868365" cy="3869186"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>124558</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>58615</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>87925</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Verbindingslijn: gebogen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C502B28B-CA5A-4B69-91D1-B117A6800898}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1398711" y="4108937"/>
+          <a:ext cx="4654062" cy="3563817"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 104127"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>102578</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>51290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>102578</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>117229</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Verbindingslijn: gebogen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA53CEAB-A78F-46B9-A091-8965A549D4EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1184033" y="4094285"/>
+          <a:ext cx="4676039" cy="3600450"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100237"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>62123</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>99392</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>124558</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Verbindingslijn: gebogen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EA353B8-0A7F-456D-A891-DBF883D34FE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="2" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="937848" y="1990058"/>
+          <a:ext cx="4100210" cy="3019008"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -7167"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>80598</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>102578</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>109904</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>124562</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Verbindingslijn: gebogen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FFD1139-9302-4B73-8AB4-DEBBD08A77A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1184397" y="2008679"/>
+          <a:ext cx="4060584" cy="3029681"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -5191"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>117233</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>80595</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>82829</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>132523</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Verbindingslijn: gebogen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52A3A365-7667-44A5-B17D-D4CC3003BEAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1560795" y="2836315"/>
+          <a:ext cx="4085559" cy="1357075"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>109904</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>65940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>117235</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>139214</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Verbindingslijn: gebogen 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A251EE93-F525-4401-8E37-61644240DB5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2677258" y="2708761"/>
+          <a:ext cx="4111874" cy="1607531"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 34356"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>87923</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>87924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>102579</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>146542</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Verbindingslijn: gebogen 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45B8064-D6B2-40A2-9B14-4E08F8FE43CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2466242" y="2719755"/>
+          <a:ext cx="4097218" cy="1614856"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -9498"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>107674</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>132524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>95252</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161194</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Verbindingslijn: gebogen 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380DD9EB-67A2-4FBF-B974-5046F62CC5E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1573856" y="3064407"/>
+          <a:ext cx="4062301" cy="981491"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 52243"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>139212</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>20513</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>165653</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>174378</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Afbeelding 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28E5FE78-9789-417B-9F97-EB3BA60B0F45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:alphaModFix amt="58000"/>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="7781225" y="617625"/>
+          <a:ext cx="1868365" cy="3855491"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>109905</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1538650" cy="2535118"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Afbeelding 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84C9569-22BD-4DA5-8CCB-7485A7161511}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:alphaModFix amt="58000"/>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="10089171" y="6030061"/>
+          <a:ext cx="2535118" cy="1538650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>41415</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>132521</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>141902</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>107674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Afbeelding 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4B4B97-2B8D-41F9-BA81-1BFD19D18C98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:alphaModFix amt="58000"/>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2849219" y="5557630"/>
+          <a:ext cx="2287096" cy="2269435"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>78950</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>168964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>115957</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>144119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Afbeelding 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BDB9E3D-2EA2-44DB-A024-379E7E1B8B4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:alphaModFix amt="58000"/>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7326233" y="5594073"/>
+          <a:ext cx="2223615" cy="2269437"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Afbeelding 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31F4F3B8-5324-47F5-9EED-6BF2201E4D4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7477125" y="3505200"/>
+          <a:ext cx="209550" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Afbeelding 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73B718CF-C8D9-46D9-9B04-9DBAB56A510D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8439978" y="5425109"/>
+          <a:ext cx="208308" cy="208308"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
@@ -1650,8 +2527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3044E5FB-7470-4B8D-8AA1-5639FB7FE80D}">
   <dimension ref="A1:BG44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BI15" sqref="BI15"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4549,4 +5426,2907 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A599D22B-B317-43DD-B1AD-3A60392861D9}">
+  <dimension ref="A1:BG44"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AC21" sqref="AC21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="3" style="1" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="33" width="3" style="1" customWidth="1"/>
+    <col min="34" max="34" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="58" width="3" style="1" customWidth="1"/>
+    <col min="59" max="59" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:59" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="J1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="AQ1" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="BB3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BF3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="BG3" s="4"/>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="1">
+        <v>18</v>
+      </c>
+      <c r="AH4" s="4">
+        <v>18</v>
+      </c>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="5"/>
+      <c r="AU4" s="5"/>
+      <c r="AV4" s="5"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="5"/>
+      <c r="AY4" s="5"/>
+      <c r="AZ4" s="5"/>
+      <c r="BA4" s="5"/>
+      <c r="BB4" s="5"/>
+      <c r="BC4" s="5"/>
+      <c r="BD4" s="5"/>
+      <c r="BE4" s="5"/>
+      <c r="BF4" s="5"/>
+      <c r="BG4" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="1">
+        <v>17</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>17</v>
+      </c>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="5"/>
+      <c r="AZ5" s="5"/>
+      <c r="BA5" s="5"/>
+      <c r="BB5" s="5"/>
+      <c r="BC5" s="5"/>
+      <c r="BD5" s="5"/>
+      <c r="BE5" s="5"/>
+      <c r="BF5" s="5"/>
+      <c r="BG5" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="1">
+        <v>16</v>
+      </c>
+      <c r="AH6" s="4">
+        <v>16</v>
+      </c>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="6"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="6"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="5"/>
+      <c r="AU6" s="6"/>
+      <c r="AW6" s="5"/>
+      <c r="AX6" s="5"/>
+      <c r="AY6" s="5"/>
+      <c r="AZ6" s="5"/>
+      <c r="BA6" s="5"/>
+      <c r="BB6" s="5"/>
+      <c r="BC6" s="5"/>
+      <c r="BD6" s="5"/>
+      <c r="BE6" s="5"/>
+      <c r="BF6" s="5"/>
+      <c r="BG6" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="24"/>
+      <c r="AA7" s="1">
+        <v>15</v>
+      </c>
+      <c r="AH7" s="4">
+        <v>15</v>
+      </c>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="10"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="11"/>
+      <c r="AM7" s="12"/>
+      <c r="AN7" s="16"/>
+      <c r="AO7" s="14"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="11"/>
+      <c r="AU7" s="15"/>
+      <c r="AV7" s="17"/>
+      <c r="AW7" s="14"/>
+      <c r="AX7" s="5"/>
+      <c r="AY7" s="5"/>
+      <c r="AZ7" s="5"/>
+      <c r="BA7" s="5"/>
+      <c r="BB7" s="5"/>
+      <c r="BC7" s="5"/>
+      <c r="BD7" s="5"/>
+      <c r="BE7" s="5"/>
+      <c r="BF7" s="5"/>
+      <c r="BG7" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="1">
+        <v>14</v>
+      </c>
+      <c r="AH8" s="4">
+        <v>14</v>
+      </c>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="5"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="5"/>
+      <c r="AU8" s="7"/>
+      <c r="AV8" s="7"/>
+      <c r="AW8" s="7"/>
+      <c r="AX8" s="5"/>
+      <c r="AY8" s="5"/>
+      <c r="AZ8" s="5"/>
+      <c r="BA8" s="5"/>
+      <c r="BB8" s="5"/>
+      <c r="BC8" s="5"/>
+      <c r="BD8" s="5"/>
+      <c r="BE8" s="5"/>
+      <c r="BF8" s="5"/>
+      <c r="BG8" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="1">
+        <v>13</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>13</v>
+      </c>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="5"/>
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="5"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="5"/>
+      <c r="AQ9" s="5"/>
+      <c r="AR9" s="5"/>
+      <c r="AS9" s="5"/>
+      <c r="AT9" s="5"/>
+      <c r="AU9" s="5"/>
+      <c r="AV9" s="5"/>
+      <c r="AW9" s="5"/>
+      <c r="AX9" s="5"/>
+      <c r="AY9" s="5"/>
+      <c r="AZ9" s="5"/>
+      <c r="BA9" s="5"/>
+      <c r="BB9" s="5"/>
+      <c r="BC9" s="5"/>
+      <c r="BD9" s="5"/>
+      <c r="BE9" s="5"/>
+      <c r="BF9" s="5"/>
+      <c r="BG9" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="1">
+        <v>12</v>
+      </c>
+      <c r="AH10" s="4">
+        <v>12</v>
+      </c>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5"/>
+      <c r="AQ10" s="5"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="5"/>
+      <c r="AU10" s="5"/>
+      <c r="AV10" s="5"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="5"/>
+      <c r="AY10" s="5"/>
+      <c r="AZ10" s="5"/>
+      <c r="BA10" s="5"/>
+      <c r="BB10" s="5"/>
+      <c r="BC10" s="5"/>
+      <c r="BD10" s="5"/>
+      <c r="BE10" s="5"/>
+      <c r="BF10" s="5"/>
+      <c r="BG10" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="1">
+        <v>11</v>
+      </c>
+      <c r="AH11" s="4">
+        <v>11</v>
+      </c>
+      <c r="AI11" s="5"/>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="5"/>
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="5"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="5"/>
+      <c r="AQ11" s="5"/>
+      <c r="AR11" s="5"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="5"/>
+      <c r="AU11" s="5"/>
+      <c r="AV11" s="5"/>
+      <c r="AW11" s="5"/>
+      <c r="AX11" s="5"/>
+      <c r="AY11" s="5"/>
+      <c r="AZ11" s="5"/>
+      <c r="BA11" s="5"/>
+      <c r="BB11" s="5"/>
+      <c r="BC11" s="5"/>
+      <c r="BD11" s="5"/>
+      <c r="BE11" s="5"/>
+      <c r="BF11" s="5"/>
+      <c r="BG11" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH12" s="4">
+        <v>10</v>
+      </c>
+      <c r="AI12" s="5"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="5"/>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="5"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="5"/>
+      <c r="AQ12" s="5"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="5"/>
+      <c r="AU12" s="5"/>
+      <c r="AV12" s="5"/>
+      <c r="AW12" s="5"/>
+      <c r="AX12" s="5"/>
+      <c r="AY12" s="5"/>
+      <c r="AZ12" s="5"/>
+      <c r="BA12" s="5"/>
+      <c r="BB12" s="5"/>
+      <c r="BC12" s="5"/>
+      <c r="BD12" s="5"/>
+      <c r="BE12" s="5"/>
+      <c r="BF12" s="5"/>
+      <c r="BG12" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="1">
+        <v>9</v>
+      </c>
+      <c r="AH13" s="4">
+        <v>9</v>
+      </c>
+      <c r="AI13" s="5"/>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="5"/>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="5"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="5"/>
+      <c r="AR13" s="5"/>
+      <c r="AS13" s="5"/>
+      <c r="AT13" s="5"/>
+      <c r="AU13" s="5"/>
+      <c r="AV13" s="5"/>
+      <c r="AW13" s="5"/>
+      <c r="AX13" s="5"/>
+      <c r="AY13" s="5"/>
+      <c r="AZ13" s="5"/>
+      <c r="BA13" s="5"/>
+      <c r="BB13" s="5"/>
+      <c r="BC13" s="5"/>
+      <c r="BD13" s="5"/>
+      <c r="BE13" s="5"/>
+      <c r="BF13" s="5"/>
+      <c r="BG13" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH14" s="4">
+        <v>8</v>
+      </c>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="5"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="5"/>
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="5"/>
+      <c r="AQ14" s="5"/>
+      <c r="AR14" s="5"/>
+      <c r="AS14" s="5"/>
+      <c r="AT14" s="5"/>
+      <c r="AU14" s="5"/>
+      <c r="AV14" s="5"/>
+      <c r="AW14" s="5"/>
+      <c r="AX14" s="5"/>
+      <c r="AY14" s="5"/>
+      <c r="AZ14" s="5"/>
+      <c r="BA14" s="5"/>
+      <c r="BB14" s="5"/>
+      <c r="BC14" s="5"/>
+      <c r="BD14" s="5"/>
+      <c r="BE14" s="5"/>
+      <c r="BF14" s="5"/>
+      <c r="BG14" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH15" s="4">
+        <v>7</v>
+      </c>
+      <c r="AI15" s="5"/>
+      <c r="AJ15" s="5"/>
+      <c r="AK15" s="5"/>
+      <c r="AL15" s="5"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="5"/>
+      <c r="AO15" s="5"/>
+      <c r="AP15" s="5"/>
+      <c r="AQ15" s="5"/>
+      <c r="AR15" s="5"/>
+      <c r="AS15" s="5"/>
+      <c r="AT15" s="5"/>
+      <c r="AU15" s="5"/>
+      <c r="AV15" s="5"/>
+      <c r="AW15" s="5"/>
+      <c r="AX15" s="5"/>
+      <c r="AY15" s="5"/>
+      <c r="AZ15" s="5"/>
+      <c r="BA15" s="5"/>
+      <c r="BB15" s="5"/>
+      <c r="BC15" s="5"/>
+      <c r="BD15" s="5"/>
+      <c r="BE15" s="5"/>
+      <c r="BF15" s="5"/>
+      <c r="BG15" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH16" s="4">
+        <v>6</v>
+      </c>
+      <c r="AI16" s="5"/>
+      <c r="AJ16" s="5"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="5"/>
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="5"/>
+      <c r="AO16" s="5"/>
+      <c r="AP16" s="5"/>
+      <c r="AQ16" s="5"/>
+      <c r="AR16" s="5"/>
+      <c r="AS16" s="5"/>
+      <c r="AT16" s="5"/>
+      <c r="AU16" s="5"/>
+      <c r="AV16" s="5"/>
+      <c r="AW16" s="5"/>
+      <c r="AX16" s="5"/>
+      <c r="AY16" s="5"/>
+      <c r="AZ16" s="5"/>
+      <c r="BA16" s="5"/>
+      <c r="BB16" s="5"/>
+      <c r="BC16" s="5"/>
+      <c r="BD16" s="5"/>
+      <c r="BE16" s="5"/>
+      <c r="BF16" s="5"/>
+      <c r="BG16" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH17" s="4">
+        <v>5</v>
+      </c>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="6"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="5"/>
+      <c r="AM17" s="5"/>
+      <c r="AN17" s="5"/>
+      <c r="AO17" s="5"/>
+      <c r="AP17" s="5"/>
+      <c r="AQ17" s="5"/>
+      <c r="AR17" s="5"/>
+      <c r="AS17" s="5"/>
+      <c r="AT17" s="6"/>
+      <c r="AU17" s="5"/>
+      <c r="AV17" s="5"/>
+      <c r="AW17" s="5"/>
+      <c r="AX17" s="5"/>
+      <c r="AY17" s="5"/>
+      <c r="AZ17" s="5"/>
+      <c r="BA17" s="5"/>
+      <c r="BB17" s="5"/>
+      <c r="BC17" s="5"/>
+      <c r="BD17" s="5"/>
+      <c r="BE17" s="5"/>
+      <c r="BF17" s="5"/>
+      <c r="BG17" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH18" s="4">
+        <v>4</v>
+      </c>
+      <c r="AI18" s="8"/>
+      <c r="AJ18" s="10"/>
+      <c r="AK18" s="9"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="5"/>
+      <c r="AQ18" s="5"/>
+      <c r="AR18" s="5"/>
+      <c r="AS18" s="11"/>
+      <c r="AT18" s="7"/>
+      <c r="AU18" s="9"/>
+      <c r="AV18" s="5"/>
+      <c r="AW18" s="5"/>
+      <c r="AX18" s="5"/>
+      <c r="AY18" s="5"/>
+      <c r="AZ18" s="5"/>
+      <c r="BA18" s="5"/>
+      <c r="BB18" s="5"/>
+      <c r="BC18" s="5"/>
+      <c r="BD18" s="5"/>
+      <c r="BE18" s="5"/>
+      <c r="BF18" s="5"/>
+      <c r="BG18" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH19" s="4">
+        <v>3</v>
+      </c>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+      <c r="AK19" s="5"/>
+      <c r="AL19" s="5"/>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="5"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="5"/>
+      <c r="AQ19" s="5"/>
+      <c r="AR19" s="5"/>
+      <c r="AS19" s="5"/>
+      <c r="AT19" s="7"/>
+      <c r="AU19" s="5"/>
+      <c r="AV19" s="5"/>
+      <c r="AW19" s="5"/>
+      <c r="AX19" s="5"/>
+      <c r="AY19" s="5"/>
+      <c r="AZ19" s="5"/>
+      <c r="BA19" s="5"/>
+      <c r="BB19" s="5"/>
+      <c r="BC19" s="5"/>
+      <c r="BD19" s="5"/>
+      <c r="BE19" s="5"/>
+      <c r="BF19" s="5"/>
+      <c r="BG19" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH20" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI20" s="5"/>
+      <c r="AJ20" s="5"/>
+      <c r="AK20" s="5"/>
+      <c r="AL20" s="5"/>
+      <c r="AM20" s="5"/>
+      <c r="AN20" s="5"/>
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="5"/>
+      <c r="AQ20" s="5"/>
+      <c r="AR20" s="5"/>
+      <c r="AS20" s="5"/>
+      <c r="AT20" s="5"/>
+      <c r="AU20" s="5"/>
+      <c r="AV20" s="5"/>
+      <c r="AW20" s="5"/>
+      <c r="AX20" s="5"/>
+      <c r="AY20" s="5"/>
+      <c r="AZ20" s="5"/>
+      <c r="BA20" s="5"/>
+      <c r="BB20" s="5"/>
+      <c r="BC20" s="5"/>
+      <c r="BD20" s="5"/>
+      <c r="BE20" s="5"/>
+      <c r="BF20" s="5"/>
+      <c r="BG20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI21" s="5"/>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="5"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="5"/>
+      <c r="AO21" s="5"/>
+      <c r="AP21" s="5"/>
+      <c r="AQ21" s="5"/>
+      <c r="AR21" s="5"/>
+      <c r="AS21" s="5"/>
+      <c r="AT21" s="5"/>
+      <c r="AU21" s="5"/>
+      <c r="AV21" s="5"/>
+      <c r="AW21" s="5"/>
+      <c r="AX21" s="5"/>
+      <c r="AY21" s="5"/>
+      <c r="AZ21" s="5"/>
+      <c r="BA21" s="5"/>
+      <c r="BB21" s="5"/>
+      <c r="BC21" s="5"/>
+      <c r="BD21" s="5"/>
+      <c r="BE21" s="5"/>
+      <c r="BF21" s="5"/>
+      <c r="BG21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="BB22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BF22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="BG22" s="4"/>
+    </row>
+    <row r="25" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BB25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BF25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>18</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="1">
+        <v>18</v>
+      </c>
+      <c r="AH26" s="1">
+        <v>18</v>
+      </c>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="2"/>
+      <c r="AN26" s="2"/>
+      <c r="AO26" s="2"/>
+      <c r="AP26" s="2"/>
+      <c r="AQ26" s="2"/>
+      <c r="AR26" s="2"/>
+      <c r="AS26" s="2"/>
+      <c r="AT26" s="2"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="2"/>
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="2"/>
+      <c r="BD26" s="2"/>
+      <c r="BE26" s="2"/>
+      <c r="BF26" s="2"/>
+      <c r="BG26" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>17</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="1">
+        <v>17</v>
+      </c>
+      <c r="AH27" s="1">
+        <v>17</v>
+      </c>
+      <c r="AI27" s="2"/>
+      <c r="AJ27" s="2"/>
+      <c r="AK27" s="2"/>
+      <c r="AL27" s="2"/>
+      <c r="AM27" s="2"/>
+      <c r="AN27" s="2"/>
+      <c r="AO27" s="2"/>
+      <c r="AP27" s="2"/>
+      <c r="AQ27" s="2"/>
+      <c r="AR27" s="2"/>
+      <c r="AS27" s="2"/>
+      <c r="AT27" s="2"/>
+      <c r="AU27" s="2"/>
+      <c r="AV27" s="2"/>
+      <c r="AW27" s="2"/>
+      <c r="AX27" s="2"/>
+      <c r="AY27" s="2"/>
+      <c r="AZ27" s="2"/>
+      <c r="BA27" s="2"/>
+      <c r="BB27" s="2"/>
+      <c r="BC27" s="2"/>
+      <c r="BD27" s="2"/>
+      <c r="BE27" s="2"/>
+      <c r="BF27" s="2"/>
+      <c r="BG27" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="2:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
+        <v>16</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="1">
+        <v>16</v>
+      </c>
+      <c r="AH28" s="1">
+        <v>16</v>
+      </c>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="2"/>
+      <c r="AK28" s="2"/>
+      <c r="AL28" s="2"/>
+      <c r="AM28" s="17"/>
+      <c r="AN28" s="15"/>
+      <c r="AO28" s="2"/>
+      <c r="AP28" s="8"/>
+      <c r="AQ28" s="2"/>
+      <c r="AR28" s="2"/>
+      <c r="AS28" s="2"/>
+      <c r="AT28" s="2"/>
+      <c r="AU28" s="2"/>
+      <c r="AV28" s="2"/>
+      <c r="AW28" s="2"/>
+      <c r="AX28" s="2"/>
+      <c r="AY28" s="2"/>
+      <c r="AZ28" s="2"/>
+      <c r="BA28" s="2"/>
+      <c r="BB28" s="12"/>
+      <c r="BC28" s="16"/>
+      <c r="BD28" s="2"/>
+      <c r="BE28" s="2"/>
+      <c r="BF28" s="2"/>
+      <c r="BG28" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>15</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="1">
+        <v>15</v>
+      </c>
+      <c r="AH29" s="1">
+        <v>15</v>
+      </c>
+      <c r="AI29" s="2"/>
+      <c r="AJ29" s="2"/>
+      <c r="AK29" s="2"/>
+      <c r="AL29" s="2"/>
+      <c r="AM29" s="2"/>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="2"/>
+      <c r="AP29" s="2"/>
+      <c r="AQ29" s="2"/>
+      <c r="AR29" s="2"/>
+      <c r="AS29" s="2"/>
+      <c r="AT29" s="2"/>
+      <c r="AU29" s="2"/>
+      <c r="AV29" s="2"/>
+      <c r="AW29" s="2"/>
+      <c r="AX29" s="2"/>
+      <c r="AY29" s="2"/>
+      <c r="AZ29" s="2"/>
+      <c r="BA29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BC29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BD29" s="2"/>
+      <c r="BE29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BF29" s="2"/>
+      <c r="BG29" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="1">
+        <v>14</v>
+      </c>
+      <c r="AH30" s="1">
+        <v>14</v>
+      </c>
+      <c r="AI30" s="2"/>
+      <c r="AJ30" s="2"/>
+      <c r="AK30" s="2"/>
+      <c r="AL30" s="2"/>
+      <c r="AM30" s="2"/>
+      <c r="AN30" s="2"/>
+      <c r="AO30" s="2"/>
+      <c r="AP30" s="2"/>
+      <c r="AQ30" s="2"/>
+      <c r="AR30" s="2"/>
+      <c r="AS30" s="2"/>
+      <c r="AT30" s="2"/>
+      <c r="AU30" s="2"/>
+      <c r="AV30" s="2"/>
+      <c r="AW30" s="2"/>
+      <c r="AX30" s="2"/>
+      <c r="AY30" s="2"/>
+      <c r="AZ30" s="2"/>
+      <c r="BA30" s="2"/>
+      <c r="BB30" s="2"/>
+      <c r="BC30" s="2"/>
+      <c r="BD30" s="2"/>
+      <c r="BE30" s="2"/>
+      <c r="BF30" s="2"/>
+      <c r="BG30" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>13</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="1">
+        <v>13</v>
+      </c>
+      <c r="AH31" s="1">
+        <v>13</v>
+      </c>
+      <c r="AI31" s="2"/>
+      <c r="AJ31" s="2"/>
+      <c r="AK31" s="2"/>
+      <c r="AL31" s="2"/>
+      <c r="AM31" s="2"/>
+      <c r="AN31" s="2"/>
+      <c r="AO31" s="2"/>
+      <c r="AP31" s="2"/>
+      <c r="AQ31" s="2"/>
+      <c r="AR31" s="2"/>
+      <c r="AS31" s="2"/>
+      <c r="AT31" s="2"/>
+      <c r="AU31" s="2"/>
+      <c r="AV31" s="2"/>
+      <c r="AW31" s="2"/>
+      <c r="AX31" s="2"/>
+      <c r="AY31" s="2"/>
+      <c r="AZ31" s="2"/>
+      <c r="BA31" s="2"/>
+      <c r="BB31" s="2"/>
+      <c r="BC31" s="2"/>
+      <c r="BD31" s="2"/>
+      <c r="BE31" s="2"/>
+      <c r="BF31" s="2"/>
+      <c r="BG31" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="2:59" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="1">
+        <v>12</v>
+      </c>
+      <c r="AH32" s="1">
+        <v>12</v>
+      </c>
+      <c r="AI32" s="2"/>
+      <c r="AJ32" s="2"/>
+      <c r="AK32" s="2"/>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="2"/>
+      <c r="AN32" s="2"/>
+      <c r="AO32" s="2"/>
+      <c r="AP32" s="2"/>
+      <c r="AQ32" s="2"/>
+      <c r="AR32" s="2"/>
+      <c r="AS32" s="2"/>
+      <c r="AT32" s="2"/>
+      <c r="AU32" s="2"/>
+      <c r="AV32" s="2"/>
+      <c r="AW32" s="2"/>
+      <c r="AX32" s="2"/>
+      <c r="AY32" s="2"/>
+      <c r="AZ32" s="2"/>
+      <c r="BA32" s="2"/>
+      <c r="BB32" s="2"/>
+      <c r="BC32" s="2"/>
+      <c r="BD32" s="2"/>
+      <c r="BE32" s="2"/>
+      <c r="BF32" s="2"/>
+      <c r="BG32" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>11</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="1">
+        <v>11</v>
+      </c>
+      <c r="AH33" s="1">
+        <v>11</v>
+      </c>
+      <c r="AI33" s="2"/>
+      <c r="AJ33" s="2"/>
+      <c r="AK33" s="2"/>
+      <c r="AL33" s="2"/>
+      <c r="AM33" s="2"/>
+      <c r="AN33" s="2"/>
+      <c r="AO33" s="2"/>
+      <c r="AP33" s="2"/>
+      <c r="AQ33" s="2"/>
+      <c r="AR33" s="2"/>
+      <c r="AS33" s="2"/>
+      <c r="AT33" s="2"/>
+      <c r="AU33" s="2"/>
+      <c r="AV33" s="2"/>
+      <c r="AW33" s="2"/>
+      <c r="AX33" s="2"/>
+      <c r="AY33" s="2"/>
+      <c r="AZ33" s="2"/>
+      <c r="BA33" s="2"/>
+      <c r="BB33" s="2"/>
+      <c r="BC33" s="2"/>
+      <c r="BD33" s="2"/>
+      <c r="BE33" s="2"/>
+      <c r="BF33" s="2"/>
+      <c r="BG33" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1">
+        <v>10</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH34" s="1">
+        <v>10</v>
+      </c>
+      <c r="AI34" s="2"/>
+      <c r="AJ34" s="2"/>
+      <c r="AK34" s="2"/>
+      <c r="AL34" s="2"/>
+      <c r="AM34" s="2"/>
+      <c r="AN34" s="2"/>
+      <c r="AO34" s="2"/>
+      <c r="AP34" s="2"/>
+      <c r="AQ34" s="2"/>
+      <c r="AR34" s="2"/>
+      <c r="AS34" s="2"/>
+      <c r="AT34" s="2"/>
+      <c r="AU34" s="2"/>
+      <c r="AV34" s="2"/>
+      <c r="AW34" s="2"/>
+      <c r="AX34" s="2"/>
+      <c r="AY34" s="2"/>
+      <c r="AZ34" s="2"/>
+      <c r="BA34" s="2"/>
+      <c r="BB34" s="2"/>
+      <c r="BC34" s="2"/>
+      <c r="BD34" s="2"/>
+      <c r="BE34" s="2"/>
+      <c r="BF34" s="2"/>
+      <c r="BG34" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="1">
+        <v>9</v>
+      </c>
+      <c r="AH35" s="1">
+        <v>9</v>
+      </c>
+      <c r="AI35" s="2"/>
+      <c r="AJ35" s="2"/>
+      <c r="AK35" s="2"/>
+      <c r="AL35" s="2"/>
+      <c r="AM35" s="2"/>
+      <c r="AN35" s="2"/>
+      <c r="AO35" s="2"/>
+      <c r="AP35" s="2"/>
+      <c r="AQ35" s="2"/>
+      <c r="AR35" s="2"/>
+      <c r="AS35" s="2"/>
+      <c r="AT35" s="2"/>
+      <c r="AU35" s="2"/>
+      <c r="AV35" s="2"/>
+      <c r="AW35" s="2"/>
+      <c r="AX35" s="2"/>
+      <c r="AY35" s="2"/>
+      <c r="AZ35" s="2"/>
+      <c r="BA35" s="2"/>
+      <c r="BB35" s="2"/>
+      <c r="BC35" s="2"/>
+      <c r="BD35" s="2"/>
+      <c r="BE35" s="2"/>
+      <c r="BF35" s="2"/>
+      <c r="BG35" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH36" s="1">
+        <v>8</v>
+      </c>
+      <c r="AI36" s="2"/>
+      <c r="AJ36" s="2"/>
+      <c r="AK36" s="2"/>
+      <c r="AL36" s="2"/>
+      <c r="AM36" s="2"/>
+      <c r="AN36" s="2"/>
+      <c r="AO36" s="2"/>
+      <c r="AP36" s="2"/>
+      <c r="AQ36" s="2"/>
+      <c r="AR36" s="2"/>
+      <c r="AS36" s="2"/>
+      <c r="AT36" s="2"/>
+      <c r="AU36" s="2"/>
+      <c r="AV36" s="2"/>
+      <c r="AW36" s="2"/>
+      <c r="AX36" s="2"/>
+      <c r="AY36" s="2"/>
+      <c r="AZ36" s="2"/>
+      <c r="BA36" s="2"/>
+      <c r="BB36" s="2"/>
+      <c r="BC36" s="2"/>
+      <c r="BD36" s="2"/>
+      <c r="BE36" s="2"/>
+      <c r="BF36" s="2"/>
+      <c r="BG36" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>7</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH37" s="1">
+        <v>7</v>
+      </c>
+      <c r="AI37" s="2"/>
+      <c r="AJ37" s="2"/>
+      <c r="AK37" s="2"/>
+      <c r="AL37" s="2"/>
+      <c r="AM37" s="2"/>
+      <c r="AN37" s="2"/>
+      <c r="AO37" s="2"/>
+      <c r="AP37" s="2"/>
+      <c r="AQ37" s="2"/>
+      <c r="AR37" s="2"/>
+      <c r="AS37" s="2"/>
+      <c r="AT37" s="2"/>
+      <c r="AU37" s="2"/>
+      <c r="AV37" s="2"/>
+      <c r="AW37" s="2"/>
+      <c r="AX37" s="2"/>
+      <c r="AY37" s="2"/>
+      <c r="AZ37" s="2"/>
+      <c r="BA37" s="2"/>
+      <c r="BB37" s="2"/>
+      <c r="BC37" s="2"/>
+      <c r="BD37" s="2"/>
+      <c r="BE37" s="2"/>
+      <c r="BF37" s="2"/>
+      <c r="BG37" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>6</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH38" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI38" s="2"/>
+      <c r="AJ38" s="2"/>
+      <c r="AK38" s="2"/>
+      <c r="AL38" s="2"/>
+      <c r="AM38" s="2"/>
+      <c r="AN38" s="2"/>
+      <c r="AO38" s="2"/>
+      <c r="AP38" s="2"/>
+      <c r="AQ38" s="2"/>
+      <c r="AR38" s="2"/>
+      <c r="AS38" s="2"/>
+      <c r="AT38" s="2"/>
+      <c r="AU38" s="2"/>
+      <c r="AV38" s="2"/>
+      <c r="AW38" s="2"/>
+      <c r="AX38" s="2"/>
+      <c r="AY38" s="2"/>
+      <c r="AZ38" s="2"/>
+      <c r="BA38" s="2"/>
+      <c r="BB38" s="2"/>
+      <c r="BC38" s="2"/>
+      <c r="BD38" s="2"/>
+      <c r="BE38" s="2"/>
+      <c r="BF38" s="2"/>
+      <c r="BG38" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH39" s="1">
+        <v>5</v>
+      </c>
+      <c r="AI39" s="2"/>
+      <c r="AJ39" s="2"/>
+      <c r="AK39" s="2"/>
+      <c r="AL39" s="2"/>
+      <c r="AM39" s="2"/>
+      <c r="AN39" s="2"/>
+      <c r="AO39" s="2"/>
+      <c r="AP39" s="2"/>
+      <c r="AQ39" s="2"/>
+      <c r="AR39" s="2"/>
+      <c r="AS39" s="2"/>
+      <c r="AT39" s="2"/>
+      <c r="AU39" s="2"/>
+      <c r="AV39" s="2"/>
+      <c r="AW39" s="2"/>
+      <c r="AX39" s="2"/>
+      <c r="AY39" s="2"/>
+      <c r="AZ39" s="2"/>
+      <c r="BA39" s="2"/>
+      <c r="BB39" s="2"/>
+      <c r="BC39" s="2"/>
+      <c r="BD39" s="2"/>
+      <c r="BE39" s="2"/>
+      <c r="BF39" s="2"/>
+      <c r="BG39" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH40" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI40" s="2"/>
+      <c r="AJ40" s="2"/>
+      <c r="AK40" s="2"/>
+      <c r="AL40" s="2"/>
+      <c r="AM40" s="2"/>
+      <c r="AN40" s="2"/>
+      <c r="AO40" s="2"/>
+      <c r="AP40" s="2"/>
+      <c r="AQ40" s="2"/>
+      <c r="AR40" s="2"/>
+      <c r="AS40" s="2"/>
+      <c r="AT40" s="2"/>
+      <c r="AU40" s="2"/>
+      <c r="AV40" s="2"/>
+      <c r="AW40" s="2"/>
+      <c r="AX40" s="2"/>
+      <c r="AY40" s="2"/>
+      <c r="AZ40" s="2"/>
+      <c r="BA40" s="2"/>
+      <c r="BB40" s="2"/>
+      <c r="BC40" s="2"/>
+      <c r="BD40" s="2"/>
+      <c r="BE40" s="2"/>
+      <c r="BF40" s="2"/>
+      <c r="BG40" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="1">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH41" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI41" s="2"/>
+      <c r="AJ41" s="2"/>
+      <c r="AK41" s="2"/>
+      <c r="AL41" s="2"/>
+      <c r="AM41" s="2"/>
+      <c r="AN41" s="2"/>
+      <c r="AO41" s="2"/>
+      <c r="AP41" s="2"/>
+      <c r="AQ41" s="2"/>
+      <c r="AR41" s="2"/>
+      <c r="AS41" s="2"/>
+      <c r="AT41" s="2"/>
+      <c r="AU41" s="2"/>
+      <c r="AV41" s="2"/>
+      <c r="AW41" s="2"/>
+      <c r="AX41" s="2"/>
+      <c r="AY41" s="2"/>
+      <c r="AZ41" s="2"/>
+      <c r="BA41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="BC41" s="2"/>
+      <c r="BD41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BE41" s="2"/>
+      <c r="BF41" s="2"/>
+      <c r="BG41" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH42" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI42" s="2"/>
+      <c r="AJ42" s="2"/>
+      <c r="AK42" s="2"/>
+      <c r="AL42" s="2"/>
+      <c r="AM42" s="2"/>
+      <c r="AN42" s="2"/>
+      <c r="AO42" s="2"/>
+      <c r="AP42" s="2"/>
+      <c r="AQ42" s="2"/>
+      <c r="AR42" s="2"/>
+      <c r="AS42" s="2"/>
+      <c r="AT42" s="2"/>
+      <c r="AU42" s="2"/>
+      <c r="AV42" s="2"/>
+      <c r="AW42" s="2"/>
+      <c r="AX42" s="2"/>
+      <c r="AY42" s="2"/>
+      <c r="AZ42" s="2"/>
+      <c r="BA42" s="8"/>
+      <c r="BB42" s="10"/>
+      <c r="BC42" s="2"/>
+      <c r="BD42" s="2"/>
+      <c r="BE42" s="2"/>
+      <c r="BF42" s="2"/>
+      <c r="BG42" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI43" s="2"/>
+      <c r="AJ43" s="2"/>
+      <c r="AK43" s="2"/>
+      <c r="AL43" s="2"/>
+      <c r="AM43" s="2"/>
+      <c r="AN43" s="2"/>
+      <c r="AO43" s="2"/>
+      <c r="AP43" s="2"/>
+      <c r="AQ43" s="2"/>
+      <c r="AR43" s="2"/>
+      <c r="AS43" s="2"/>
+      <c r="AT43" s="2"/>
+      <c r="AU43" s="2"/>
+      <c r="AV43" s="2"/>
+      <c r="AW43" s="2"/>
+      <c r="AX43" s="2"/>
+      <c r="AY43" s="2"/>
+      <c r="AZ43" s="2"/>
+      <c r="BA43" s="2"/>
+      <c r="BB43" s="2"/>
+      <c r="BC43" s="2"/>
+      <c r="BD43" s="2"/>
+      <c r="BE43" s="2"/>
+      <c r="BF43" s="2"/>
+      <c r="BG43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BB44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="BD44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BF44" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>